<commit_message>
fft hip example with inplace transpose
</commit_message>
<xml_diff>
--- a/fft/inplace transpose.xlsx
+++ b/fft/inplace transpose.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\fft_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\rocm_start_sample\fft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEFAE8D-E4EA-44FB-8529-B4E90BB12DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC3B8B5-A2C7-47B1-A813-45512621FE3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="16">
   <si>
     <t>mask=0110</t>
   </si>
@@ -289,7 +290,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -567,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q11" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AY17" sqref="AY17"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM58" sqref="AM58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1916,7 +1928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -1947,53 +1959,868 @@
       <c r="AC33" s="19"/>
       <c r="AD33" s="19"/>
     </row>
-    <row r="34" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="9">
+        <v>2</v>
+      </c>
+      <c r="G40" s="10">
+        <v>3</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="6">
+        <v>13</v>
+      </c>
+      <c r="M40" s="17">
+        <v>14</v>
+      </c>
+      <c r="N40" s="18">
+        <v>15</v>
+      </c>
+      <c r="R40" s="3">
+        <v>0</v>
+      </c>
+      <c r="S40" s="6">
+        <v>13</v>
+      </c>
+      <c r="T40" s="15">
+        <v>10</v>
+      </c>
+      <c r="U40" s="14">
+        <v>11</v>
+      </c>
+      <c r="Y40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="6">
+        <v>13</v>
+      </c>
+      <c r="AA40" s="15">
+        <v>10</v>
+      </c>
+      <c r="AB40" s="13">
+        <v>7</v>
+      </c>
+      <c r="AF40" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG40" s="17">
+        <v>13</v>
+      </c>
+      <c r="AH40" s="15">
+        <v>10</v>
+      </c>
+      <c r="AI40" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="11">
+        <v>4</v>
+      </c>
+      <c r="E41" s="4">
+        <v>5</v>
+      </c>
+      <c r="F41" s="12">
+        <v>6</v>
+      </c>
+      <c r="G41" s="13">
+        <v>7</v>
+      </c>
+      <c r="K41" s="11">
+        <v>4</v>
+      </c>
+      <c r="L41" s="7">
+        <v>1</v>
+      </c>
+      <c r="M41" s="9">
+        <v>2</v>
+      </c>
+      <c r="N41" s="10">
+        <v>3</v>
+      </c>
+      <c r="R41" s="11">
+        <v>4</v>
+      </c>
+      <c r="S41" s="7">
+        <v>1</v>
+      </c>
+      <c r="T41" s="17">
+        <v>14</v>
+      </c>
+      <c r="U41" s="18">
+        <v>15</v>
+      </c>
+      <c r="Y41" s="11">
+        <v>4</v>
+      </c>
+      <c r="Z41" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="17">
+        <v>14</v>
+      </c>
+      <c r="AB41" s="14">
+        <v>11</v>
+      </c>
+      <c r="AF41" s="12">
+        <v>4</v>
+      </c>
+      <c r="AG41" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH41" s="17">
+        <v>14</v>
+      </c>
+      <c r="AI41" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="5">
+        <v>8</v>
+      </c>
+      <c r="E42" s="8">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15">
+        <v>10</v>
+      </c>
+      <c r="G42" s="14">
+        <v>11</v>
+      </c>
+      <c r="K42" s="5">
+        <v>8</v>
+      </c>
+      <c r="L42" s="4">
+        <v>5</v>
+      </c>
+      <c r="M42" s="12">
+        <v>6</v>
+      </c>
+      <c r="N42" s="13">
+        <v>7</v>
+      </c>
+      <c r="R42" s="5">
+        <v>8</v>
+      </c>
+      <c r="S42" s="4">
+        <v>5</v>
+      </c>
+      <c r="T42" s="9">
+        <v>2</v>
+      </c>
+      <c r="U42" s="10">
+        <v>3</v>
+      </c>
+      <c r="Y42" s="5">
+        <v>8</v>
+      </c>
+      <c r="Z42" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA42" s="9">
+        <v>2</v>
+      </c>
+      <c r="AB42" s="18">
+        <v>15</v>
+      </c>
+      <c r="AF42" s="15">
+        <v>8</v>
+      </c>
+      <c r="AG42" s="12">
+        <v>5</v>
+      </c>
+      <c r="AH42" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI42" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="16">
+        <v>12</v>
+      </c>
+      <c r="E43" s="6">
+        <v>13</v>
+      </c>
+      <c r="F43" s="17">
+        <v>14</v>
+      </c>
+      <c r="G43" s="18">
+        <v>15</v>
+      </c>
+      <c r="K43" s="16">
+        <v>12</v>
+      </c>
+      <c r="L43" s="8">
+        <v>9</v>
+      </c>
+      <c r="M43" s="15">
+        <v>10</v>
+      </c>
+      <c r="N43" s="14">
+        <v>11</v>
+      </c>
+      <c r="R43" s="16">
+        <v>12</v>
+      </c>
+      <c r="S43" s="8">
+        <v>9</v>
+      </c>
+      <c r="T43" s="12">
+        <v>6</v>
+      </c>
+      <c r="U43" s="13">
+        <v>7</v>
+      </c>
+      <c r="Y43" s="16">
+        <v>12</v>
+      </c>
+      <c r="Z43" s="8">
+        <v>9</v>
+      </c>
+      <c r="AA43" s="12">
+        <v>6</v>
+      </c>
+      <c r="AB43" s="10">
+        <v>3</v>
+      </c>
+      <c r="AF43" s="17">
+        <v>12</v>
+      </c>
+      <c r="AG43" s="15">
+        <v>9</v>
+      </c>
+      <c r="AH43" s="12">
+        <v>6</v>
+      </c>
+      <c r="AI43" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AK44" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AK45" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y46" s="19"/>
+      <c r="Z46" s="19"/>
+      <c r="AA46" s="19"/>
+      <c r="AB46" s="19"/>
+      <c r="AF46" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG46" s="17">
+        <v>13</v>
+      </c>
+      <c r="AH46" s="15">
+        <v>10</v>
+      </c>
+      <c r="AI46" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="19"/>
+      <c r="AA47" s="19"/>
+      <c r="AB47" s="19"/>
+      <c r="AF47" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="12">
+        <v>4</v>
+      </c>
+      <c r="AH47" s="17">
+        <v>14</v>
+      </c>
+      <c r="AI47" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="19"/>
+      <c r="AA48" s="19"/>
+      <c r="AB48" s="19"/>
+      <c r="AF48" s="15">
+        <v>8</v>
+      </c>
+      <c r="AG48" s="12">
+        <v>5</v>
+      </c>
+      <c r="AH48" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI48" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y49" s="19"/>
+      <c r="Z49" s="19"/>
+      <c r="AA49" s="19"/>
+      <c r="AB49" s="19"/>
+      <c r="AF49" s="15">
+        <v>9</v>
+      </c>
+      <c r="AG49" s="17">
+        <v>12</v>
+      </c>
+      <c r="AH49" s="12">
+        <v>6</v>
+      </c>
+      <c r="AI49" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AK50" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y51" s="19"/>
+      <c r="Z51" s="19"/>
+      <c r="AA51" s="19"/>
+      <c r="AB51" s="19"/>
+      <c r="AC51" s="19"/>
+      <c r="AE51" s="19"/>
+      <c r="AF51" s="19"/>
+      <c r="AG51" s="19"/>
+      <c r="AH51" s="19"/>
+      <c r="AI51" s="19"/>
+      <c r="AJ51" s="19"/>
+      <c r="AK51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO51" s="19"/>
+      <c r="AP51" s="19"/>
+      <c r="AQ51" s="19"/>
+      <c r="AR51" s="19"/>
+    </row>
+    <row r="52" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y52" s="19"/>
+      <c r="Z52" s="19"/>
+      <c r="AA52" s="19"/>
+      <c r="AB52" s="19"/>
+      <c r="AC52" s="19"/>
+      <c r="AD52" s="19"/>
+      <c r="AE52" s="19"/>
+      <c r="AF52" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG52" s="17">
+        <v>13</v>
+      </c>
+      <c r="AH52" s="15">
+        <v>10</v>
+      </c>
+      <c r="AI52" s="12">
+        <v>7</v>
+      </c>
+      <c r="AJ52" s="19"/>
+      <c r="AO52" s="19"/>
+      <c r="AP52" s="19"/>
+      <c r="AQ52" s="19"/>
+      <c r="AR52" s="19"/>
+    </row>
+    <row r="53" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y53" s="19"/>
+      <c r="Z53" s="19"/>
+      <c r="AA53" s="19"/>
+      <c r="AB53" s="19"/>
+      <c r="AC53" s="19"/>
+      <c r="AD53" s="19"/>
+      <c r="AE53" s="19"/>
+      <c r="AF53" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG53" s="12">
+        <v>4</v>
+      </c>
+      <c r="AH53" s="15">
+        <v>11</v>
+      </c>
+      <c r="AI53" s="17">
+        <v>14</v>
+      </c>
+      <c r="AJ53" s="19"/>
+      <c r="AO53" s="19"/>
+      <c r="AP53" s="19"/>
+      <c r="AQ53" s="19"/>
+      <c r="AR53" s="19"/>
+    </row>
+    <row r="54" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y54" s="19"/>
+      <c r="Z54" s="19"/>
+      <c r="AA54" s="19"/>
+      <c r="AB54" s="19"/>
+      <c r="AC54" s="19"/>
+      <c r="AD54" s="19"/>
+      <c r="AE54" s="19"/>
+      <c r="AF54" s="15">
+        <v>8</v>
+      </c>
+      <c r="AG54" s="12">
+        <v>5</v>
+      </c>
+      <c r="AH54" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI54" s="17">
+        <v>15</v>
+      </c>
+      <c r="AJ54" s="19"/>
+      <c r="AO54" s="19"/>
+      <c r="AP54" s="19"/>
+      <c r="AQ54" s="19"/>
+      <c r="AR54" s="19"/>
+    </row>
+    <row r="55" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y55" s="19"/>
+      <c r="Z55" s="19"/>
+      <c r="AA55" s="19"/>
+      <c r="AB55" s="19"/>
+      <c r="AC55" s="19"/>
+      <c r="AD55" s="19"/>
+      <c r="AE55" s="19"/>
+      <c r="AF55" s="15">
+        <v>9</v>
+      </c>
+      <c r="AG55" s="17">
+        <v>12</v>
+      </c>
+      <c r="AH55" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI55" s="12">
+        <v>6</v>
+      </c>
+      <c r="AJ55" s="19"/>
+    </row>
+    <row r="56" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y56" s="19"/>
+      <c r="Z56" s="19"/>
+      <c r="AA56" s="19"/>
+      <c r="AB56" s="19"/>
+      <c r="AC56" s="19"/>
+      <c r="AD56" s="19"/>
+      <c r="AE56" s="19"/>
+      <c r="AF56" s="19"/>
+      <c r="AG56" s="19"/>
+      <c r="AH56" s="19"/>
+      <c r="AI56" s="19"/>
+      <c r="AJ56" s="19"/>
+      <c r="AK56" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y57" s="19"/>
+      <c r="Z57" s="19"/>
+      <c r="AA57" s="19"/>
+      <c r="AB57" s="19"/>
+      <c r="AC57" s="19"/>
+      <c r="AD57" s="19"/>
+      <c r="AE57" s="19"/>
+      <c r="AF57" s="19"/>
+      <c r="AG57" s="19"/>
+      <c r="AH57" s="19"/>
+      <c r="AI57" s="19"/>
+      <c r="AJ57" s="19"/>
+      <c r="AK57" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y58" s="19"/>
+      <c r="Z58" s="19"/>
+      <c r="AA58" s="19"/>
+      <c r="AB58" s="19"/>
+      <c r="AC58" s="19"/>
+      <c r="AD58" s="19"/>
+      <c r="AE58" s="19"/>
+      <c r="AF58" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG58" s="12">
+        <v>7</v>
+      </c>
+      <c r="AH58" s="15">
+        <v>10</v>
+      </c>
+      <c r="AI58" s="17">
+        <v>13</v>
+      </c>
+      <c r="AJ58" s="19"/>
+    </row>
+    <row r="59" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y59" s="19"/>
+      <c r="Z59" s="19"/>
+      <c r="AA59" s="19"/>
+      <c r="AB59" s="19"/>
+      <c r="AC59" s="19"/>
+      <c r="AD59" s="19"/>
+      <c r="AE59" s="19"/>
+      <c r="AF59" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG59" s="12">
+        <v>4</v>
+      </c>
+      <c r="AH59" s="15">
+        <v>11</v>
+      </c>
+      <c r="AI59" s="17">
+        <v>14</v>
+      </c>
+      <c r="AJ59" s="19"/>
+    </row>
+    <row r="60" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y60" s="19"/>
+      <c r="Z60" s="19"/>
+      <c r="AA60" s="19"/>
+      <c r="AB60" s="19"/>
+      <c r="AC60" s="19"/>
+      <c r="AD60" s="19"/>
+      <c r="AE60" s="19"/>
+      <c r="AF60" s="15">
+        <v>8</v>
+      </c>
+      <c r="AG60" s="12">
+        <v>5</v>
+      </c>
+      <c r="AH60" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI60" s="17">
+        <v>15</v>
+      </c>
+      <c r="AJ60" s="19"/>
+    </row>
+    <row r="61" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y61" s="19"/>
+      <c r="Z61" s="19"/>
+      <c r="AA61" s="19"/>
+      <c r="AB61" s="19"/>
+      <c r="AC61" s="19"/>
+      <c r="AD61" s="19"/>
+      <c r="AE61" s="19"/>
+      <c r="AF61" s="15">
+        <v>9</v>
+      </c>
+      <c r="AG61" s="12">
+        <v>6</v>
+      </c>
+      <c r="AH61" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI61" s="17">
+        <v>12</v>
+      </c>
+      <c r="AJ61" s="19"/>
+    </row>
+    <row r="62" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y62" s="19"/>
+      <c r="Z62" s="19"/>
+      <c r="AA62" s="19"/>
+      <c r="AB62" s="19"/>
+      <c r="AK62" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y63" s="19"/>
+      <c r="Z63" s="19"/>
+      <c r="AA63" s="19"/>
+      <c r="AB63" s="19"/>
+      <c r="AK63" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="4:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="11">
+        <v>4</v>
+      </c>
+      <c r="F64" s="5">
+        <v>8</v>
+      </c>
+      <c r="G64" s="16">
+        <v>12</v>
+      </c>
+      <c r="K64" s="3">
+        <v>0</v>
+      </c>
+      <c r="L64" s="11">
+        <v>4</v>
+      </c>
+      <c r="M64" s="5">
+        <v>8</v>
+      </c>
+      <c r="N64" s="18">
+        <v>15</v>
+      </c>
+      <c r="R64" s="3">
+        <v>0</v>
+      </c>
+      <c r="S64" s="11">
+        <v>4</v>
+      </c>
+      <c r="T64" s="14">
+        <v>11</v>
+      </c>
+      <c r="U64" s="17">
+        <v>14</v>
+      </c>
+      <c r="Y64" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="13">
+        <v>7</v>
+      </c>
+      <c r="AA64" s="15">
+        <v>10</v>
+      </c>
+      <c r="AB64" s="6">
+        <v>13</v>
+      </c>
+      <c r="AF64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="12">
+        <v>7</v>
+      </c>
+      <c r="AH64" s="15">
+        <v>10</v>
+      </c>
+      <c r="AI64" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D65" s="7">
+        <v>1</v>
+      </c>
+      <c r="E65" s="4">
+        <v>5</v>
+      </c>
+      <c r="F65" s="8">
+        <v>9</v>
+      </c>
+      <c r="G65" s="6">
+        <v>13</v>
+      </c>
+      <c r="K65" s="7">
+        <v>1</v>
+      </c>
+      <c r="L65" s="4">
+        <v>5</v>
+      </c>
+      <c r="M65" s="8">
+        <v>9</v>
+      </c>
+      <c r="N65" s="16">
+        <v>12</v>
+      </c>
+      <c r="R65" s="7">
+        <v>1</v>
+      </c>
+      <c r="S65" s="4">
+        <v>5</v>
+      </c>
+      <c r="T65" s="5">
+        <v>8</v>
+      </c>
+      <c r="U65" s="18">
+        <v>15</v>
+      </c>
+      <c r="Y65" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z65" s="11">
+        <v>4</v>
+      </c>
+      <c r="AA65" s="14">
+        <v>11</v>
+      </c>
+      <c r="AB65" s="17">
+        <v>14</v>
+      </c>
+      <c r="AF65" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG65" s="12">
+        <v>4</v>
+      </c>
+      <c r="AH65" s="15">
+        <v>11</v>
+      </c>
+      <c r="AI65" s="17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D66" s="9">
+        <v>2</v>
+      </c>
+      <c r="E66" s="12">
+        <v>6</v>
+      </c>
+      <c r="F66" s="15">
+        <v>10</v>
+      </c>
+      <c r="G66" s="17">
+        <v>14</v>
+      </c>
+      <c r="K66" s="9">
+        <v>2</v>
+      </c>
+      <c r="L66" s="12">
+        <v>6</v>
+      </c>
+      <c r="M66" s="15">
+        <v>10</v>
+      </c>
+      <c r="N66" s="6">
+        <v>13</v>
+      </c>
+      <c r="R66" s="9">
+        <v>2</v>
+      </c>
+      <c r="S66" s="12">
+        <v>6</v>
+      </c>
+      <c r="T66" s="8">
+        <v>9</v>
+      </c>
+      <c r="U66" s="16">
+        <v>12</v>
+      </c>
+      <c r="Y66" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z66" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA66" s="5">
+        <v>8</v>
+      </c>
+      <c r="AB66" s="18">
+        <v>15</v>
+      </c>
+      <c r="AF66" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG66" s="12">
+        <v>5</v>
+      </c>
+      <c r="AH66" s="15">
+        <v>8</v>
+      </c>
+      <c r="AI66" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D67" s="10">
+        <v>3</v>
+      </c>
+      <c r="E67" s="13">
+        <v>7</v>
+      </c>
+      <c r="F67" s="14">
+        <v>11</v>
+      </c>
+      <c r="G67" s="18">
+        <v>15</v>
+      </c>
+      <c r="K67" s="10">
+        <v>3</v>
+      </c>
+      <c r="L67" s="13">
+        <v>7</v>
+      </c>
+      <c r="M67" s="14">
+        <v>11</v>
+      </c>
+      <c r="N67" s="17">
+        <v>14</v>
+      </c>
+      <c r="R67" s="10">
+        <v>3</v>
+      </c>
+      <c r="S67" s="13">
+        <v>7</v>
+      </c>
+      <c r="T67" s="15">
+        <v>10</v>
+      </c>
+      <c r="U67" s="6">
+        <v>13</v>
+      </c>
+      <c r="Y67" s="10">
+        <v>3</v>
+      </c>
+      <c r="Z67" s="12">
+        <v>6</v>
+      </c>
+      <c r="AA67" s="8">
+        <v>9</v>
+      </c>
+      <c r="AB67" s="16">
+        <v>12</v>
+      </c>
+      <c r="AF67" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG67" s="12">
+        <v>6</v>
+      </c>
+      <c r="AH67" s="15">
+        <v>9</v>
+      </c>
+      <c r="AI67" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="71" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="73" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="4:35" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="81" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="82" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2064,6 +2891,9 @@
     <row r="148" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="Y46:AB50">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
@@ -2073,6 +2903,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96130B77-A7B7-4CA1-A8E0-1CE3815B63A7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;11&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB62146-96DC-4411-9B41-7CE78F764A64}">
   <dimension ref="C1:AG180"/>
   <sheetViews>

</xml_diff>